<commit_message>
Added code to create extra spreadsheets for Capstone data
</commit_message>
<xml_diff>
--- a/Testing Files/Processor Test Files/HatcoMLSDataTestingSmall.xlsx
+++ b/Testing Files/Processor Test Files/HatcoMLSDataTestingSmall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Origami1105\source\repos\HatcoMarketShareHelper\Testing Files\Processor Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31F47016-EA17-44C8-9782-E51CBEF64609}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90B7A56-8162-405F-B70A-58110D2783BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2614,7 +2614,7 @@
   <dimension ref="A1:N151"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E148" sqref="E148"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>